<commit_message>
rework lab №2 and otchet
</commit_message>
<xml_diff>
--- a/Lab/02/data.xlsx
+++ b/Lab/02/data.xlsx
@@ -461,7 +461,7 @@
         </is>
       </c>
       <c r="C2" s="1" t="n">
-        <v>44192.92946427388</v>
+        <v>44208.76488976447</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="C3" s="1" t="n">
-        <v>44192.92946427388</v>
+        <v>44208.76488976447</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>

</xml_diff>